<commit_message>
Agregado template equipos/home.html en la ruta correcta
</commit_message>
<xml_diff>
--- a/Maquinaria/equipos.xlsx
+++ b/Maquinaria/equipos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maquinaria\Maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313806A6-7929-4A13-A580-A9FF0B7FFA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF26E62C-D09F-48DF-8BDA-C312023D17EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F849151E-99BA-4359-88C9-4C85D25037A7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="220">
   <si>
     <t>FORD</t>
   </si>
@@ -694,6 +694,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>VBDV-10</t>
   </si>
 </sst>
 </file>
@@ -1104,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD361ED-4A05-4D9F-85E5-097DB587E69C}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1133,7 +1136,7 @@
       <c r="C1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>209</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -1150,60 +1153,60 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
+      <c r="A2" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>9</v>
       </c>
       <c r="D2" s="8">
+        <v>2025</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
         <v>2022</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2021</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -1212,24 +1215,24 @@
         <v>1</v>
       </c>
       <c r="D4" s="8">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -1244,18 +1247,18 @@
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
@@ -1264,24 +1267,24 @@
         <v>1</v>
       </c>
       <c r="D6" s="8">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
@@ -1296,18 +1299,18 @@
         <v>0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
@@ -1322,18 +1325,18 @@
         <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
@@ -1342,24 +1345,24 @@
         <v>1</v>
       </c>
       <c r="D9" s="8">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
@@ -1377,41 +1380,41 @@
         <v>29</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2025</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6">
-        <v>2</v>
-      </c>
-      <c r="D11" s="8">
-        <v>2020</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="4">
-        <v>266172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
@@ -1420,186 +1423,186 @@
         <v>2</v>
       </c>
       <c r="D12" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="4">
+        <v>266172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8">
         <v>2019</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
         <v>5</v>
-      </c>
-      <c r="D13" s="8">
-        <v>2023</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>7</v>
       </c>
       <c r="D14" s="8">
         <v>2023</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>215</v>
+        <v>49</v>
       </c>
       <c r="B15" s="6">
         <v>1</v>
       </c>
       <c r="C15" s="6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D15" s="8">
         <v>2023</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2023</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="4">
         <v>4080547</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6">
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
         <v>10</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D17" s="8">
         <v>2024</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H17" s="4">
         <v>107941</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
         <v>2</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D18" s="8">
         <v>2025</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
         <v>4</v>
-      </c>
-      <c r="D18" s="8">
-        <v>2024</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="4">
-        <v>2927624</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="6">
-        <v>15</v>
       </c>
       <c r="D19" s="8">
         <v>2024</v>
@@ -1608,70 +1611,70 @@
         <v>63</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G19" s="4">
-        <v>2736422</v>
+        <v>2927624</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>15</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2024</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2736422</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="6">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6">
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6">
         <v>8</v>
-      </c>
-      <c r="D20" s="8">
-        <v>2025</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="6">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6">
-        <v>9</v>
       </c>
       <c r="D21" s="8">
         <v>2025</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
@@ -1686,18 +1689,18 @@
         <v>39</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B23" s="6">
         <v>1</v>
@@ -1712,44 +1715,44 @@
         <v>39</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6">
+        <v>9</v>
+      </c>
+      <c r="D24" s="8">
+        <v>2025</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B24" s="6">
-        <v>1</v>
-      </c>
-      <c r="C24" s="6">
-        <v>12</v>
-      </c>
-      <c r="D24" s="8">
-        <v>2019</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="4">
-        <v>320</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="B25" s="6">
         <v>1</v>
@@ -1758,76 +1761,76 @@
         <v>12</v>
       </c>
       <c r="D25" s="8">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F25" s="4">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>88</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>89</v>
+      <c r="A26" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B26" s="6">
         <v>1</v>
       </c>
       <c r="C26" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" s="8">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F26" s="4">
-        <v>140</v>
+        <v>330</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B27" s="6">
         <v>1</v>
       </c>
       <c r="C27" s="6">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D27" s="8">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
+      </c>
+      <c r="F27" s="4">
+        <v>140</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B28" s="6">
         <v>1</v>
@@ -1836,50 +1839,50 @@
         <v>16</v>
       </c>
       <c r="D28" s="8">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>92</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>218</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B29" s="6">
         <v>1</v>
       </c>
       <c r="C29" s="6">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D29" s="8">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H29" s="4">
-        <v>26887431</v>
+        <v>99</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
@@ -1888,30 +1891,30 @@
         <v>11</v>
       </c>
       <c r="D30" s="8">
-        <v>2025</v>
+        <v>2021</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>218</v>
+        <v>103</v>
+      </c>
+      <c r="H30" s="4">
+        <v>26887431</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B31" s="6">
         <v>1</v>
       </c>
       <c r="C31" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" s="8">
         <v>2025</v>
@@ -1919,25 +1922,25 @@
       <c r="E31" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F31" s="4">
-        <v>330</v>
+      <c r="F31" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B32" s="6">
         <v>1</v>
       </c>
       <c r="C32" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D32" s="8">
         <v>2025</v>
@@ -1946,76 +1949,76 @@
         <v>83</v>
       </c>
       <c r="F32" s="4">
-        <v>966</v>
+        <v>330</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B33" s="6">
         <v>1</v>
       </c>
       <c r="C33" s="6">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D33" s="8">
         <v>2025</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>115</v>
+        <v>83</v>
+      </c>
+      <c r="F33" s="4">
+        <v>966</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B34" s="6">
         <v>1</v>
       </c>
       <c r="C34" s="6">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D34" s="8">
         <v>2025</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F34" s="4">
-        <v>330</v>
+        <v>113</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B35" s="6">
         <v>1</v>
       </c>
       <c r="C35" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35" s="8">
         <v>2025</v>
@@ -2024,114 +2027,114 @@
         <v>83</v>
       </c>
       <c r="F35" s="4">
-        <v>966</v>
+        <v>330</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>218</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <v>11</v>
+      </c>
+      <c r="D36" s="8">
+        <v>2025</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="4">
+        <v>966</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="6">
-        <v>1</v>
-      </c>
-      <c r="C36" s="6">
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
         <v>17</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D37" s="8">
         <v>2026</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H37" s="3">
         <v>13303320</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="6">
-        <v>2</v>
-      </c>
-      <c r="C37" s="6">
-        <v>7</v>
-      </c>
-      <c r="D37" s="9">
-        <v>2023</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
       <c r="B38" s="6">
         <v>2</v>
       </c>
       <c r="C38" s="6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D38" s="9">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>218</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>134</v>
+        <v>216</v>
       </c>
       <c r="B39" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" s="6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D39" s="9">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>218</v>
@@ -2139,85 +2142,85 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B40" s="6">
         <v>3</v>
       </c>
       <c r="C40" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" s="9">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F40" s="2">
-        <v>330</v>
+      <c r="F40" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>139</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B41" s="6">
         <v>3</v>
       </c>
       <c r="C41" s="6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D41" s="9">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>141</v>
+      <c r="F41" s="2">
+        <v>330</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B42" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D42" s="9">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B43" s="6">
         <v>4</v>
@@ -2235,15 +2238,15 @@
         <v>147</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B44" s="6">
         <v>4</v>
@@ -2261,93 +2264,93 @@
         <v>147</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B45" s="6">
         <v>4</v>
       </c>
       <c r="C45" s="6">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D45" s="9">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G45" s="2">
-        <v>40332</v>
+        <v>147</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B46" s="6">
         <v>4</v>
       </c>
       <c r="C46" s="6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D46" s="9">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
+      </c>
+      <c r="G46" s="2">
+        <v>40332</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B47" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" s="6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D47" s="9">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B48" s="6">
         <v>5</v>
@@ -2362,96 +2365,96 @@
         <v>163</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B49" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D49" s="9">
-        <v>2018</v>
+        <v>2024</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B50" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" s="6">
         <v>3</v>
       </c>
       <c r="D50" s="9">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B51" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C51" s="6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D51" s="9">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B52" s="6">
         <v>8</v>
@@ -2460,24 +2463,24 @@
         <v>9</v>
       </c>
       <c r="D52" s="9">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B53" s="6">
         <v>8</v>
@@ -2486,148 +2489,174 @@
         <v>9</v>
       </c>
       <c r="D53" s="9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>187</v>
+        <v>80</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>191</v>
+      <c r="A54" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="B54" s="6">
         <v>8</v>
       </c>
-      <c r="C54" s="7">
-        <v>6</v>
-      </c>
-      <c r="D54" s="8">
-        <v>2020</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>194</v>
+      <c r="C54" s="6">
+        <v>9</v>
+      </c>
+      <c r="D54" s="9">
+        <v>2024</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>195</v>
+      <c r="A55" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="B55" s="6">
         <v>8</v>
       </c>
-      <c r="C55" s="6">
-        <v>9</v>
-      </c>
-      <c r="D55" s="9">
-        <v>2025</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>198</v>
+      <c r="C55" s="7">
+        <v>6</v>
+      </c>
+      <c r="D55" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B56" s="6">
         <v>8</v>
       </c>
       <c r="C56" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D56" s="9">
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="B57" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C57" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D57" s="9">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58" s="6">
+        <v>9</v>
+      </c>
+      <c r="C58" s="6">
+        <v>3</v>
+      </c>
+      <c r="D58" s="9">
+        <v>2016</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B59" s="6">
         <v>10</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C59" s="6">
         <v>18</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D59" s="9">
         <v>2023</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>206</v>
       </c>
     </row>

</xml_diff>